<commit_message>
updated documentation and index.razor
</commit_message>
<xml_diff>
--- a/Documents/Mini svendeprøve projekt Gantt diagram.xlsx
+++ b/Documents/Mini svendeprøve projekt Gantt diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Mercantec\H5\Mini-svendeproeve-projekt\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ACC293-78DC-41E7-9F3B-AA644335EFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5720CF04-8555-4AC4-8AF7-759D40D99CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsplan før arbejde" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Process</t>
   </si>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -584,6 +584,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -591,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39D23B6-9CEB-4EC0-A503-C500F87A7AFD}">
   <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,6 +684,12 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -707,5 +714,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>